<commit_message>
ReadList : Add finding strategies
</commit_message>
<xml_diff>
--- a/ReadState.xlsx
+++ b/ReadState.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giamberm\Documents\TI\paper\2_Anomalie-detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702A0B4D-E09F-4377-834B-6E0A7E63579E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B32F878-B6AA-44C0-B31D-FDBE78B144BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="375" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
   <si>
     <t>Start</t>
   </si>
@@ -126,6 +126,18 @@
   </si>
   <si>
     <t>DAGMM</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>ReaschGate, Anomaly detection review</t>
+  </si>
+  <si>
+    <t>Anomaly detection unsupervised multivariate</t>
+  </si>
+  <si>
+    <t>sciencedirect, "anomaly detection" "unsupervised", review, 2010-2022</t>
   </si>
 </sst>
 </file>
@@ -176,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -191,11 +203,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,15 +495,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:P53"/>
+  <dimension ref="C7:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
     <col min="6" max="6" width="107.140625" bestFit="1" customWidth="1"/>
@@ -497,36 +516,37 @@
     <col min="16" max="16" width="10" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2">
-        <f>COUNTIF(D11:D1000,D11)</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H7" s="3">
         <f ca="1">NOW()</f>
-        <v>45373.416640162039</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="H9" s="6" t="s">
+        <v>45373.677645833333</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1">
+        <f>COUNTIF(D11:D1000,D11)</f>
+        <v>18</v>
+      </c>
+      <c r="H9" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="6"/>
-      <c r="K9" s="6" t="s">
+      <c r="I9" s="8"/>
+      <c r="K9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="L9" s="6"/>
-      <c r="N9" s="6" t="s">
+      <c r="L9" s="8"/>
+      <c r="N9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="O9" s="6"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O9" s="8"/>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="D10" s="2" t="s">
         <v>26</v>
       </c>
@@ -567,8 +587,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="7" t="s">
+    <row r="11" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="1">
@@ -600,8 +623,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D12" s="7" t="s">
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C12" s="9"/>
+      <c r="D12" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="1">
@@ -633,8 +657,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D13" s="7" t="s">
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C13" s="9"/>
+      <c r="D13" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E13" s="1">
@@ -666,8 +691,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D14" s="7" t="s">
+    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C14" s="9"/>
+      <c r="D14" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E14" s="1">
@@ -703,8 +729,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D15" s="7" t="s">
+    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C15" s="9"/>
+      <c r="D15" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E15" s="1">
@@ -736,8 +763,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D16" s="7" t="s">
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C16" s="9"/>
+      <c r="D16" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E16" s="1">
@@ -769,8 +797,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D17" s="7" t="s">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C17" s="9"/>
+      <c r="D17" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E17" s="1">
@@ -802,8 +831,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D18" s="7" t="s">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C18" s="9"/>
+      <c r="D18" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E18" s="1">
@@ -838,8 +868,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D19" s="7" t="s">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C19" s="9"/>
+      <c r="D19" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E19" s="1">
@@ -874,8 +905,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D20" s="7" t="s">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C20" s="9"/>
+      <c r="D20" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E20" s="1">
@@ -910,8 +942,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D21" s="7" t="s">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C21" s="6"/>
+      <c r="D21" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E21" s="1">
@@ -946,7 +979,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C22" s="6"/>
       <c r="D22" t="s">
         <v>29</v>
       </c>
@@ -982,8 +1016,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D23" s="7" t="s">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C23" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E23" s="1">
@@ -1018,8 +1055,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D24" s="7" t="s">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C24" s="9"/>
+      <c r="D24" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E24" s="1">
@@ -1054,8 +1092,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D25" s="7" t="s">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C25" s="9"/>
+      <c r="D25" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E25" s="1">
@@ -1090,7 +1129,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C26" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="1">
+        <v>16</v>
+      </c>
+      <c r="F26" s="1"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="K26" s="3"/>
@@ -1098,7 +1147,14 @@
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
     </row>
-    <row r="27" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C27" s="9"/>
+      <c r="D27" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="1">
+        <v>17</v>
+      </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="K27" s="3"/>
@@ -1106,7 +1162,14 @@
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
     </row>
-    <row r="28" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C28" s="9"/>
+      <c r="D28" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="1">
+        <v>18</v>
+      </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="K28" s="3"/>
@@ -1114,7 +1177,14 @@
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
     </row>
-    <row r="29" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C29" s="9"/>
+      <c r="D29" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="1">
+        <v>19</v>
+      </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="K29" s="3"/>
@@ -1122,7 +1192,14 @@
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
     </row>
-    <row r="30" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C30" s="9"/>
+      <c r="D30" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="1">
+        <v>20</v>
+      </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="K30" s="3"/>
@@ -1130,7 +1207,7 @@
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
     </row>
-    <row r="31" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="K31" s="3"/>
@@ -1138,7 +1215,7 @@
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
     </row>
-    <row r="32" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="K32" s="3"/>
@@ -1315,10 +1392,13 @@
       <c r="O53" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="N9:O9"/>
+    <mergeCell ref="C11:C20"/>
+    <mergeCell ref="C26:C30"/>
+    <mergeCell ref="C23:C25"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:D1000" xr:uid="{3C1CE3FE-DB2C-4C19-8BC4-C9EF203C546F}">

</xml_diff>

<commit_message>
ReadState.xlsx : reading on unsupervised anomaly detection review
</commit_message>
<xml_diff>
--- a/ReadState.xlsx
+++ b/ReadState.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giamberm\Documents\TI\paper\2_Anomalie-detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B32F878-B6AA-44C0-B31D-FDBE78B144BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5048279E-7FA9-4803-B827-21CA31F4A50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="375" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
   <si>
     <t>Start</t>
   </si>
@@ -138,6 +138,39 @@
   </si>
   <si>
     <t>sciencedirect, "anomaly detection" "unsupervised", review, 2010-2022</t>
+  </si>
+  <si>
+    <t>relevant</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>A survey on anomaly detection for technical systems using LSTM networks - 2021 - Lindemann</t>
+  </si>
+  <si>
+    <t>Autoencoders for unsupervised anomaly segmentation in brain MR images: A comparative study - 2021 - Baur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A deep hypersphere approach to high-dimensional anomaly detection - 2022 - Zheng </t>
+  </si>
+  <si>
+    <t>Real-time big data processing for anomaly detection: A Survey - Ahamed - 2019</t>
+  </si>
+  <si>
+    <t>A deep encoder-decoder network for anomaly detection - 2022 - Yu</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>NR</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -147,8 +180,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -188,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -214,6 +255,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -495,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C7:P53"/>
+  <dimension ref="C1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,23 +556,45 @@
     <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="64.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="107.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="1" customWidth="1"/>
-    <col min="8" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" style="1" customWidth="1"/>
-    <col min="11" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10" style="1" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="107.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="1" customWidth="1"/>
+    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" style="1" customWidth="1"/>
+    <col min="12" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="H7" s="3">
+    <row r="1" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="G1"/>
+    </row>
+    <row r="2" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="G2"/>
+    </row>
+    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="G3"/>
+    </row>
+    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="G4"/>
+    </row>
+    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="G6"/>
+    </row>
+    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="G7"/>
+      <c r="I7" s="3">
         <f ca="1">NOW()</f>
-        <v>45373.677645833333</v>
-      </c>
-    </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+        <v>45376.417222685188</v>
+      </c>
+    </row>
+    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="G8"/>
+    </row>
+    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C9" s="7" t="s">
         <v>27</v>
       </c>
@@ -530,20 +602,21 @@
         <f>COUNTIF(D11:D1000,D11)</f>
         <v>18</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="G9"/>
+      <c r="I9" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="8"/>
-      <c r="K9" s="8" t="s">
+      <c r="J9" s="8"/>
+      <c r="L9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="L9" s="8"/>
-      <c r="N9" s="8" t="s">
+      <c r="M9" s="8"/>
+      <c r="O9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="O9" s="8"/>
-    </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P9" s="8"/>
+    </row>
+    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>30</v>
       </c>
@@ -554,40 +627,43 @@
         <v>25</v>
       </c>
       <c r="F10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>0</v>
-      </c>
       <c r="I10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="5" t="s">
-        <v>0</v>
-      </c>
       <c r="L10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="N10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N10" s="5" t="s">
-        <v>0</v>
-      </c>
       <c r="O10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="Q10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="9" t="s">
         <v>31</v>
       </c>
@@ -597,33 +673,36 @@
       <c r="E11" s="1">
         <v>1</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="3">
+      <c r="I11" s="3">
         <v>45362.4377662037</v>
       </c>
-      <c r="I11" s="3">
+      <c r="J11" s="3">
         <v>45362.466927546295</v>
       </c>
-      <c r="J11" s="4">
-        <f t="shared" ref="J11:J25" si="0">I11-H11</f>
+      <c r="K11" s="4">
+        <f t="shared" ref="K11:K30" si="0">J11-I11</f>
         <v>2.9161342594306916E-2</v>
       </c>
-      <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="4">
-        <f>L11-K11</f>
-        <v>0</v>
-      </c>
-      <c r="N11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="4">
+        <f>M11-L11</f>
+        <v>0</v>
+      </c>
       <c r="O11" s="3"/>
-      <c r="P11" s="4">
-        <f>O11-N11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P11" s="3"/>
+      <c r="Q11" s="4">
+        <f>P11-O11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C12" s="9"/>
       <c r="D12" s="6" t="s">
         <v>28</v>
@@ -631,33 +710,36 @@
       <c r="E12" s="1">
         <v>2</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="3">
+      <c r="I12" s="3">
         <v>45362.588587962964</v>
       </c>
-      <c r="I12" s="3">
+      <c r="J12" s="3">
         <v>45362.615472685182</v>
       </c>
-      <c r="J12" s="4">
+      <c r="K12" s="4">
         <f t="shared" si="0"/>
         <v>2.6884722217801027E-2</v>
       </c>
-      <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="4">
-        <f t="shared" ref="M12:M25" si="1">L12-K12</f>
-        <v>0</v>
-      </c>
-      <c r="N12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="4">
+        <f t="shared" ref="N12:N30" si="1">M12-L12</f>
+        <v>0</v>
+      </c>
       <c r="O12" s="3"/>
-      <c r="P12" s="4">
-        <f t="shared" ref="P12:P13" si="2">O12-N12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P12" s="3"/>
+      <c r="Q12" s="4">
+        <f t="shared" ref="Q12:Q13" si="2">P12-O12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C13" s="9"/>
       <c r="D13" s="6" t="s">
         <v>28</v>
@@ -665,33 +747,36 @@
       <c r="E13" s="1">
         <v>3</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="3">
+      <c r="I13" s="3">
         <v>45362.637543171295</v>
       </c>
-      <c r="I13" s="3">
+      <c r="J13" s="3">
         <v>45362.646111226852</v>
       </c>
-      <c r="J13" s="4">
+      <c r="K13" s="4">
         <f t="shared" si="0"/>
         <v>8.5680555566796102E-3</v>
       </c>
-      <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O13" s="3"/>
-      <c r="P13" s="4">
+      <c r="P13" s="3"/>
+      <c r="Q13" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C14" s="9"/>
       <c r="D14" s="6" t="s">
         <v>28</v>
@@ -699,37 +784,40 @@
       <c r="E14" s="1">
         <v>4</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="3">
+      <c r="I14" s="3">
         <v>45362.651693402775</v>
       </c>
-      <c r="I14" s="3">
+      <c r="J14" s="3">
         <v>45362.66130925926</v>
       </c>
-      <c r="J14" s="4">
+      <c r="K14" s="4">
         <f t="shared" si="0"/>
         <v>9.6158564847428352E-3</v>
       </c>
-      <c r="K14" s="3">
+      <c r="L14" s="3">
         <v>45362.642175925925</v>
       </c>
-      <c r="L14" s="3">
+      <c r="M14" s="3">
         <v>45362.683872106485</v>
       </c>
-      <c r="M14" s="4">
+      <c r="N14" s="4">
         <f t="shared" si="1"/>
         <v>4.1696180560393259E-2</v>
       </c>
-      <c r="N14" s="3"/>
       <c r="O14" s="3"/>
-      <c r="P14" s="4">
-        <f>O14-N14</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P14" s="3"/>
+      <c r="Q14" s="4">
+        <f>P14-O14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C15" s="9"/>
       <c r="D15" s="6" t="s">
         <v>28</v>
@@ -737,33 +825,36 @@
       <c r="E15" s="1">
         <v>5</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="3">
+      <c r="I15" s="3">
         <v>45363.563067129631</v>
       </c>
-      <c r="I15" s="3">
+      <c r="J15" s="3">
         <v>45363.588067129633</v>
       </c>
-      <c r="J15" s="4">
+      <c r="K15" s="4">
         <f t="shared" si="0"/>
         <v>2.5000000001455192E-2</v>
       </c>
-      <c r="K15" s="3"/>
       <c r="L15" s="3"/>
-      <c r="M15" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O15" s="3"/>
-      <c r="P15" s="4">
-        <f t="shared" ref="P15:P25" si="3">O15-N15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P15" s="3"/>
+      <c r="Q15" s="4">
+        <f t="shared" ref="Q15:Q30" si="3">P15-O15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C16" s="9"/>
       <c r="D16" s="6" t="s">
         <v>28</v>
@@ -771,33 +862,36 @@
       <c r="E16" s="1">
         <v>6</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="3">
+      <c r="I16" s="3">
         <v>45363.602375462964</v>
       </c>
-      <c r="I16" s="3">
+      <c r="J16" s="3">
         <v>45363.647005208331</v>
       </c>
-      <c r="J16" s="4">
+      <c r="K16" s="4">
         <f t="shared" si="0"/>
         <v>4.4629745367274154E-2</v>
       </c>
-      <c r="K16" s="3"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O16" s="3"/>
-      <c r="P16" s="4">
+      <c r="P16" s="3"/>
+      <c r="Q16" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C17" s="9"/>
       <c r="D17" s="6" t="s">
         <v>28</v>
@@ -805,33 +899,34 @@
       <c r="E17" s="1">
         <v>7</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="9"/>
+      <c r="G17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="3">
+      <c r="I17" s="3">
         <v>45363.665852314814</v>
       </c>
-      <c r="I17" s="3">
+      <c r="J17" s="3">
         <v>45363.68843263889</v>
       </c>
-      <c r="J17" s="4">
+      <c r="K17" s="4">
         <f t="shared" si="0"/>
         <v>2.2580324075534008E-2</v>
       </c>
-      <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O17" s="3"/>
-      <c r="P17" s="4">
+      <c r="P17" s="3"/>
+      <c r="Q17" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C18" s="9"/>
       <c r="D18" s="6" t="s">
         <v>28</v>
@@ -839,36 +934,39 @@
       <c r="E18" s="1">
         <v>8</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <v>6</v>
       </c>
-      <c r="H18" s="3">
+      <c r="I18" s="3">
         <v>45365.446338078706</v>
       </c>
-      <c r="I18" s="3">
+      <c r="J18" s="3">
         <v>45365.45198946759</v>
       </c>
-      <c r="J18" s="4">
+      <c r="K18" s="4">
         <f t="shared" si="0"/>
         <v>5.6513888848712668E-3</v>
       </c>
-      <c r="K18" s="3"/>
       <c r="L18" s="3"/>
-      <c r="M18" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O18" s="3"/>
-      <c r="P18" s="4">
+      <c r="P18" s="3"/>
+      <c r="Q18" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C19" s="9"/>
       <c r="D19" s="6" t="s">
         <v>28</v>
@@ -876,36 +974,41 @@
       <c r="E19" s="1">
         <v>9</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <v>23</v>
       </c>
-      <c r="H19" s="3">
+      <c r="I19" s="3">
         <v>45365.458979166666</v>
       </c>
-      <c r="I19" s="3">
+      <c r="J19" s="3">
         <v>45365.49157604167</v>
       </c>
-      <c r="J19" s="4">
+      <c r="K19" s="4">
         <f t="shared" si="0"/>
         <v>3.2596875003946479E-2</v>
       </c>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N19" s="3"/>
+      <c r="L19" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="M19" s="12"/>
+      <c r="N19" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="O19" s="3"/>
-      <c r="P19" s="4">
+      <c r="P19" s="3"/>
+      <c r="Q19" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C20" s="9"/>
       <c r="D20" s="6" t="s">
         <v>28</v>
@@ -913,36 +1016,39 @@
       <c r="E20" s="1">
         <v>10</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H20" s="1">
         <v>14</v>
       </c>
-      <c r="H20" s="3">
+      <c r="I20" s="3">
         <v>45365.571219675927</v>
       </c>
-      <c r="I20" s="3">
+      <c r="J20" s="3">
         <v>45365.585367361113</v>
       </c>
-      <c r="J20" s="4">
+      <c r="K20" s="4">
         <f t="shared" si="0"/>
         <v>1.4147685185889713E-2</v>
       </c>
-      <c r="K20" s="3"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O20" s="3"/>
-      <c r="P20" s="4">
+      <c r="P20" s="3"/>
+      <c r="Q20" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C21" s="6"/>
       <c r="D21" s="6" t="s">
         <v>29</v>
@@ -950,36 +1056,39 @@
       <c r="E21" s="1">
         <v>11</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H21" s="1">
         <v>19</v>
       </c>
-      <c r="H21" s="3">
+      <c r="I21" s="3">
         <v>45372.411581944441</v>
       </c>
-      <c r="I21" s="3">
+      <c r="J21" s="3">
         <v>45372.437949189814</v>
       </c>
-      <c r="J21" s="4">
+      <c r="K21" s="4">
         <f t="shared" si="0"/>
         <v>2.6367245372966863E-2</v>
       </c>
-      <c r="K21" s="3"/>
       <c r="L21" s="3"/>
-      <c r="M21" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O21" s="3"/>
-      <c r="P21" s="4">
+      <c r="P21" s="3"/>
+      <c r="Q21" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C22" s="6"/>
       <c r="D22" t="s">
         <v>29</v>
@@ -987,36 +1096,39 @@
       <c r="E22" s="1">
         <v>12</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H22" s="1">
         <v>26</v>
       </c>
-      <c r="H22" s="3">
+      <c r="I22" s="3">
         <v>45372.4569505787</v>
       </c>
-      <c r="I22" s="3">
+      <c r="J22" s="3">
         <v>45372.491233449073</v>
       </c>
-      <c r="J22" s="4">
+      <c r="K22" s="4">
         <f t="shared" si="0"/>
         <v>3.428287037240807E-2</v>
       </c>
-      <c r="K22" s="3"/>
       <c r="L22" s="3"/>
-      <c r="M22" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O22" s="3"/>
-      <c r="P22" s="4">
+      <c r="P22" s="3"/>
+      <c r="Q22" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C23" s="9" t="s">
         <v>32</v>
       </c>
@@ -1026,36 +1138,39 @@
       <c r="E23" s="1">
         <v>13</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H23" s="1">
         <v>18</v>
       </c>
-      <c r="H23" s="3">
+      <c r="I23" s="3">
         <v>45372.574540162037</v>
       </c>
-      <c r="I23" s="3">
+      <c r="J23" s="3">
         <v>45372.60127673611</v>
       </c>
-      <c r="J23" s="4">
+      <c r="K23" s="4">
         <f t="shared" si="0"/>
         <v>2.6736574072856456E-2</v>
       </c>
-      <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O23" s="3"/>
-      <c r="P23" s="4">
+      <c r="P23" s="3"/>
+      <c r="Q23" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C24" s="9"/>
       <c r="D24" s="6" t="s">
         <v>28</v>
@@ -1063,36 +1178,39 @@
       <c r="E24" s="1">
         <v>14</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G24" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G24" s="1">
+      <c r="H24" s="1">
         <v>21</v>
       </c>
-      <c r="H24" s="3">
+      <c r="I24" s="3">
         <v>45372.60597060185</v>
       </c>
-      <c r="I24" s="3">
+      <c r="J24" s="3">
         <v>45372.618298611109</v>
       </c>
-      <c r="J24" s="4">
+      <c r="K24" s="4">
         <f t="shared" si="0"/>
         <v>1.2328009259363171E-2</v>
       </c>
-      <c r="K24" s="3"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O24" s="3"/>
-      <c r="P24" s="4">
+      <c r="P24" s="3"/>
+      <c r="Q24" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C25" s="9"/>
       <c r="D25" s="6" t="s">
         <v>28</v>
@@ -1100,36 +1218,39 @@
       <c r="E25" s="1">
         <v>15</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
         <v>10</v>
       </c>
-      <c r="H25" s="3">
+      <c r="I25" s="3">
         <v>45372.624619097223</v>
       </c>
-      <c r="I25" s="3">
+      <c r="J25" s="3">
         <v>45372.644125347222</v>
       </c>
-      <c r="J25" s="4">
+      <c r="K25" s="4">
         <f t="shared" si="0"/>
         <v>1.9506249998812564E-2</v>
       </c>
-      <c r="K25" s="3"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O25" s="3"/>
-      <c r="P25" s="4">
+      <c r="P25" s="3"/>
+      <c r="Q25" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C26" s="9" t="s">
         <v>33</v>
       </c>
@@ -1139,15 +1260,39 @@
       <c r="E26" s="1">
         <v>16</v>
       </c>
-      <c r="F26" s="1"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="K26" s="3"/>
+      <c r="F26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H26" s="1">
+        <v>11</v>
+      </c>
+      <c r="I26" s="3">
+        <v>45376.341631944444</v>
+      </c>
+      <c r="J26" s="3">
+        <v>45376.348576388889</v>
+      </c>
+      <c r="K26" s="4">
+        <f t="shared" si="0"/>
+        <v>6.9444444452528842E-3</v>
+      </c>
       <c r="L26" s="3"/>
-      <c r="N26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O26" s="3"/>
-    </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P26" s="3"/>
+      <c r="Q26" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C27" s="9"/>
       <c r="D27" s="6" t="s">
         <v>28</v>
@@ -1155,14 +1300,39 @@
       <c r="E27" s="1">
         <v>17</v>
       </c>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="K27" s="3"/>
+      <c r="F27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" s="1">
+        <v>16</v>
+      </c>
+      <c r="I27" s="3">
+        <v>45376.358473958331</v>
+      </c>
+      <c r="J27" s="3">
+        <v>45376.360679513891</v>
+      </c>
+      <c r="K27" s="4">
+        <f t="shared" si="0"/>
+        <v>2.205555560067296E-3</v>
+      </c>
       <c r="L27" s="3"/>
-      <c r="N27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O27" s="3"/>
-    </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P27" s="3"/>
+      <c r="Q27" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C28" s="9"/>
       <c r="D28" s="6" t="s">
         <v>28</v>
@@ -1170,14 +1340,39 @@
       <c r="E28" s="1">
         <v>18</v>
       </c>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="K28" s="3"/>
+      <c r="F28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H28" s="1">
+        <v>17</v>
+      </c>
+      <c r="I28" s="3">
+        <v>45376.3614087963</v>
+      </c>
+      <c r="J28" s="3">
+        <v>45376.367887037035</v>
+      </c>
+      <c r="K28" s="4">
+        <f t="shared" si="0"/>
+        <v>6.4782407353050075E-3</v>
+      </c>
       <c r="L28" s="3"/>
-      <c r="N28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O28" s="3"/>
-    </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P28" s="3"/>
+      <c r="Q28" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C29" s="9"/>
       <c r="D29" s="6" t="s">
         <v>28</v>
@@ -1185,14 +1380,39 @@
       <c r="E29" s="1">
         <v>19</v>
       </c>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="K29" s="3"/>
+      <c r="F29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H29" s="1">
+        <v>19</v>
+      </c>
+      <c r="I29" s="3">
+        <v>45376.376967708333</v>
+      </c>
+      <c r="J29" s="3">
+        <v>45376.380903240744</v>
+      </c>
+      <c r="K29" s="4">
+        <f t="shared" si="0"/>
+        <v>3.9355324115604162E-3</v>
+      </c>
       <c r="L29" s="3"/>
-      <c r="N29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O29" s="3"/>
-    </row>
-    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P29" s="3"/>
+      <c r="Q29" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C30" s="9"/>
       <c r="D30" s="6" t="s">
         <v>28</v>
@@ -1200,209 +1420,239 @@
       <c r="E30" s="1">
         <v>20</v>
       </c>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="K30" s="3"/>
+      <c r="F30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H30" s="1">
+        <v>16</v>
+      </c>
+      <c r="I30" s="3">
+        <v>45376.392687615742</v>
+      </c>
+      <c r="J30" s="3">
+        <v>45376.395459837964</v>
+      </c>
+      <c r="K30" s="4">
+        <f t="shared" si="0"/>
+        <v>2.7722222221200354E-3</v>
+      </c>
       <c r="L30" s="3"/>
-      <c r="N30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O30" s="3"/>
-    </row>
-    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="H31" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="3:17" x14ac:dyDescent="0.25">
       <c r="I31" s="3"/>
-      <c r="K31" s="3"/>
+      <c r="J31" s="3"/>
       <c r="L31" s="3"/>
-      <c r="N31" s="3"/>
+      <c r="M31" s="3"/>
       <c r="O31" s="3"/>
-    </row>
-    <row r="32" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="H32" s="3"/>
+      <c r="P31" s="3"/>
+    </row>
+    <row r="32" spans="3:17" x14ac:dyDescent="0.25">
       <c r="I32" s="3"/>
-      <c r="K32" s="3"/>
+      <c r="J32" s="3"/>
       <c r="L32" s="3"/>
-      <c r="N32" s="3"/>
+      <c r="M32" s="3"/>
       <c r="O32" s="3"/>
-    </row>
-    <row r="33" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H33" s="3"/>
+      <c r="P32" s="3"/>
+    </row>
+    <row r="33" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I33" s="3"/>
-      <c r="K33" s="3"/>
+      <c r="J33" s="3"/>
       <c r="L33" s="3"/>
-      <c r="N33" s="3"/>
+      <c r="M33" s="3"/>
       <c r="O33" s="3"/>
-    </row>
-    <row r="34" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H34" s="3"/>
+      <c r="P33" s="3"/>
+    </row>
+    <row r="34" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I34" s="3"/>
-      <c r="K34" s="3"/>
+      <c r="J34" s="3"/>
       <c r="L34" s="3"/>
-      <c r="N34" s="3"/>
+      <c r="M34" s="3"/>
       <c r="O34" s="3"/>
-    </row>
-    <row r="35" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H35" s="3"/>
+      <c r="P34" s="3"/>
+    </row>
+    <row r="35" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I35" s="3"/>
-      <c r="K35" s="3"/>
+      <c r="J35" s="3"/>
       <c r="L35" s="3"/>
-      <c r="N35" s="3"/>
+      <c r="M35" s="3"/>
       <c r="O35" s="3"/>
-    </row>
-    <row r="36" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H36" s="3"/>
+      <c r="P35" s="3"/>
+    </row>
+    <row r="36" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I36" s="3"/>
-      <c r="K36" s="3"/>
+      <c r="J36" s="3"/>
       <c r="L36" s="3"/>
-      <c r="N36" s="3"/>
+      <c r="M36" s="3"/>
       <c r="O36" s="3"/>
-    </row>
-    <row r="37" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H37" s="3"/>
+      <c r="P36" s="3"/>
+    </row>
+    <row r="37" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I37" s="3"/>
-      <c r="K37" s="3"/>
+      <c r="J37" s="3"/>
       <c r="L37" s="3"/>
-      <c r="N37" s="3"/>
+      <c r="M37" s="3"/>
       <c r="O37" s="3"/>
-    </row>
-    <row r="38" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H38" s="3"/>
+      <c r="P37" s="3"/>
+    </row>
+    <row r="38" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I38" s="3"/>
-      <c r="K38" s="3"/>
+      <c r="J38" s="3"/>
       <c r="L38" s="3"/>
-      <c r="N38" s="3"/>
+      <c r="M38" s="3"/>
       <c r="O38" s="3"/>
-    </row>
-    <row r="39" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H39" s="3"/>
+      <c r="P38" s="3"/>
+    </row>
+    <row r="39" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I39" s="3"/>
-      <c r="K39" s="3"/>
+      <c r="J39" s="3"/>
       <c r="L39" s="3"/>
-      <c r="N39" s="3"/>
+      <c r="M39" s="3"/>
       <c r="O39" s="3"/>
-    </row>
-    <row r="40" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H40" s="3"/>
+      <c r="P39" s="3"/>
+    </row>
+    <row r="40" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I40" s="3"/>
-      <c r="K40" s="3"/>
+      <c r="J40" s="3"/>
       <c r="L40" s="3"/>
-      <c r="N40" s="3"/>
+      <c r="M40" s="3"/>
       <c r="O40" s="3"/>
-    </row>
-    <row r="41" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H41" s="3"/>
+      <c r="P40" s="3"/>
+    </row>
+    <row r="41" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I41" s="3"/>
-      <c r="K41" s="3"/>
+      <c r="J41" s="3"/>
       <c r="L41" s="3"/>
-      <c r="N41" s="3"/>
+      <c r="M41" s="3"/>
       <c r="O41" s="3"/>
-    </row>
-    <row r="42" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H42" s="3"/>
+      <c r="P41" s="3"/>
+    </row>
+    <row r="42" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I42" s="3"/>
-      <c r="K42" s="3"/>
+      <c r="J42" s="3"/>
       <c r="L42" s="3"/>
-      <c r="N42" s="3"/>
+      <c r="M42" s="3"/>
       <c r="O42" s="3"/>
-    </row>
-    <row r="43" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H43" s="3"/>
+      <c r="P42" s="3"/>
+    </row>
+    <row r="43" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I43" s="3"/>
-      <c r="K43" s="3"/>
+      <c r="J43" s="3"/>
       <c r="L43" s="3"/>
-      <c r="N43" s="3"/>
+      <c r="M43" s="3"/>
       <c r="O43" s="3"/>
-    </row>
-    <row r="44" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H44" s="3"/>
+      <c r="P43" s="3"/>
+    </row>
+    <row r="44" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I44" s="3"/>
-      <c r="K44" s="3"/>
+      <c r="J44" s="3"/>
       <c r="L44" s="3"/>
-      <c r="N44" s="3"/>
+      <c r="M44" s="3"/>
       <c r="O44" s="3"/>
-    </row>
-    <row r="45" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H45" s="3"/>
+      <c r="P44" s="3"/>
+    </row>
+    <row r="45" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I45" s="3"/>
-      <c r="K45" s="3"/>
+      <c r="J45" s="3"/>
       <c r="L45" s="3"/>
-      <c r="N45" s="3"/>
+      <c r="M45" s="3"/>
       <c r="O45" s="3"/>
-    </row>
-    <row r="46" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H46" s="3"/>
+      <c r="P45" s="3"/>
+    </row>
+    <row r="46" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I46" s="3"/>
-      <c r="K46" s="3"/>
+      <c r="J46" s="3"/>
       <c r="L46" s="3"/>
-      <c r="N46" s="3"/>
+      <c r="M46" s="3"/>
       <c r="O46" s="3"/>
-    </row>
-    <row r="47" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H47" s="3"/>
+      <c r="P46" s="3"/>
+    </row>
+    <row r="47" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I47" s="3"/>
-      <c r="K47" s="3"/>
+      <c r="J47" s="3"/>
       <c r="L47" s="3"/>
-      <c r="N47" s="3"/>
+      <c r="M47" s="3"/>
       <c r="O47" s="3"/>
-    </row>
-    <row r="48" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H48" s="3"/>
+      <c r="P47" s="3"/>
+    </row>
+    <row r="48" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I48" s="3"/>
-      <c r="K48" s="3"/>
+      <c r="J48" s="3"/>
       <c r="L48" s="3"/>
-      <c r="N48" s="3"/>
+      <c r="M48" s="3"/>
       <c r="O48" s="3"/>
-    </row>
-    <row r="49" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H49" s="3"/>
+      <c r="P48" s="3"/>
+    </row>
+    <row r="49" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I49" s="3"/>
-      <c r="K49" s="3"/>
+      <c r="J49" s="3"/>
       <c r="L49" s="3"/>
-      <c r="N49" s="3"/>
+      <c r="M49" s="3"/>
       <c r="O49" s="3"/>
-    </row>
-    <row r="50" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H50" s="3"/>
+      <c r="P49" s="3"/>
+    </row>
+    <row r="50" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I50" s="3"/>
-      <c r="K50" s="3"/>
+      <c r="J50" s="3"/>
       <c r="L50" s="3"/>
-      <c r="N50" s="3"/>
+      <c r="M50" s="3"/>
       <c r="O50" s="3"/>
-    </row>
-    <row r="51" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H51" s="3"/>
+      <c r="P50" s="3"/>
+    </row>
+    <row r="51" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I51" s="3"/>
-      <c r="K51" s="3"/>
+      <c r="J51" s="3"/>
       <c r="L51" s="3"/>
-      <c r="N51" s="3"/>
+      <c r="M51" s="3"/>
       <c r="O51" s="3"/>
-    </row>
-    <row r="52" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H52" s="3"/>
+      <c r="P51" s="3"/>
+    </row>
+    <row r="52" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I52" s="3"/>
-      <c r="K52" s="3"/>
+      <c r="J52" s="3"/>
       <c r="L52" s="3"/>
-      <c r="N52" s="3"/>
+      <c r="M52" s="3"/>
       <c r="O52" s="3"/>
-    </row>
-    <row r="53" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H53" s="3"/>
+      <c r="P52" s="3"/>
+    </row>
+    <row r="53" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I53" s="3"/>
-      <c r="K53" s="3"/>
+      <c r="J53" s="3"/>
       <c r="L53" s="3"/>
-      <c r="N53" s="3"/>
+      <c r="M53" s="3"/>
       <c r="O53" s="3"/>
+      <c r="P53" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="N9:O9"/>
+  <mergeCells count="8">
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="O9:P9"/>
     <mergeCell ref="C11:C20"/>
     <mergeCell ref="C26:C30"/>
     <mergeCell ref="C23:C25"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="L19:M19"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:D1000" xr:uid="{3C1CE3FE-DB2C-4C19-8BC4-C9EF203C546F}">
       <formula1>$D$11:$D$1000</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:F16 F18:F1048576" xr:uid="{14583326-801D-4BAD-968B-E6609AB5FF26}">
+      <formula1>"Y, N, NR, -"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Working report KW11-13 (FR)
</commit_message>
<xml_diff>
--- a/ReadState.xlsx
+++ b/ReadState.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giamberm\Documents\TI\paper\2_Anomalie-detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104FDFF4-D4A8-458D-A85C-174FF3DF36F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DB4BA2-4866-4E40-BC69-32C7994C5E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="48">
   <si>
     <t>Start</t>
   </si>
@@ -92,15 +92,9 @@
     <t>#pages</t>
   </si>
   <si>
-    <t xml:space="preserve">Deep Learning for Anomaly Detection in Time-Series Data - 2021 - KUKJIN </t>
-  </si>
-  <si>
     <t>An Experimental Evaluation of Anomaly Detection in Time - 2023 - Zhang</t>
   </si>
   <si>
-    <t>Pyramid reconstruction assisted deep autoencoding Gaussian mixture model for industrial fault detection - 2023 - Ying</t>
-  </si>
-  <si>
     <t>DEEP AUTOENCODING GAUSSIAN MIXTURE MODEL FOR UNSUPERVISED ANOMALY DETECTION - 2018 - Zong</t>
   </si>
   <si>
@@ -171,6 +165,21 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>Not relevant</t>
+  </si>
+  <si>
+    <t>Not a review</t>
+  </si>
+  <si>
+    <t>Yes, relevant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deep Learning for Anomaly Detection in Time-Series Data - 2021 - Choi </t>
+  </si>
+  <si>
+    <t>Pyramid reconstruction assisted deep autoencoding Gaussian mixture model for industrial fault detection - 2023 - Tian</t>
   </si>
 </sst>
 </file>
@@ -547,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,24 +588,41 @@
       <c r="G4"/>
     </row>
     <row r="5" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="G5"/>
+      <c r="F5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="G6"/>
+      <c r="F6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="7" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="G7"/>
+      <c r="F7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
+        <v>45</v>
+      </c>
       <c r="I7" s="3">
         <f ca="1">NOW()</f>
-        <v>45376.728793981485</v>
+        <v>45377.426842245368</v>
       </c>
     </row>
     <row r="8" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="G8"/>
+      <c r="F8" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="9" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C9" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1">
         <f>COUNTIF(D11:D1000,D11)</f>
@@ -618,16 +644,16 @@
     </row>
     <row r="10" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>5</v>
@@ -665,16 +691,16 @@
     </row>
     <row r="11" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>9</v>
@@ -705,13 +731,13 @@
     <row r="12" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C12" s="11"/>
       <c r="D12" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E12" s="1">
         <v>2</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>11</v>
@@ -742,13 +768,13 @@
     <row r="13" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C13" s="11"/>
       <c r="D13" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E13" s="1">
         <v>3</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>10</v>
@@ -779,13 +805,13 @@
     <row r="14" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C14" s="11"/>
       <c r="D14" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E14" s="1">
         <v>4</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>12</v>
@@ -820,13 +846,13 @@
     <row r="15" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C15" s="11"/>
       <c r="D15" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E15" s="1">
         <v>5</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>13</v>
@@ -857,13 +883,13 @@
     <row r="16" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C16" s="11"/>
       <c r="D16" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E16" s="1">
         <v>6</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>14</v>
@@ -894,7 +920,7 @@
     <row r="17" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C17" s="11"/>
       <c r="D17" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E17" s="1">
         <v>7</v>
@@ -929,13 +955,13 @@
     <row r="18" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C18" s="11"/>
       <c r="D18" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E18" s="1">
         <v>8</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>16</v>
@@ -969,16 +995,16 @@
     <row r="19" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C19" s="11"/>
       <c r="D19" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E19" s="1">
         <v>9</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="H19" s="1">
         <v>23</v>
@@ -994,7 +1020,7 @@
         <v>3.2596875003946479E-2</v>
       </c>
       <c r="L19" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M19" s="12"/>
       <c r="N19" s="4" t="e">
@@ -1011,16 +1037,16 @@
     <row r="20" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C20" s="11"/>
       <c r="D20" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E20" s="1">
         <v>10</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H20" s="1">
         <v>14</v>
@@ -1051,16 +1077,16 @@
     <row r="21" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C21" s="6"/>
       <c r="D21" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E21" s="1">
         <v>11</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H21" s="1">
         <v>19</v>
@@ -1091,16 +1117,16 @@
     <row r="22" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C22" s="6"/>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E22" s="1">
         <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="H22" s="1">
         <v>26</v>
@@ -1130,19 +1156,19 @@
     </row>
     <row r="23" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C23" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E23" s="1">
         <v>13</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H23" s="1">
         <v>18</v>
@@ -1173,16 +1199,16 @@
     <row r="24" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C24" s="11"/>
       <c r="D24" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E24" s="1">
         <v>14</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H24" s="1">
         <v>21</v>
@@ -1213,16 +1239,16 @@
     <row r="25" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C25" s="11"/>
       <c r="D25" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E25" s="1">
         <v>15</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H25" s="1">
         <v>10</v>
@@ -1252,19 +1278,19 @@
     </row>
     <row r="26" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C26" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E26" s="1">
         <v>16</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H26" s="1">
         <v>11</v>
@@ -1295,16 +1321,16 @@
     <row r="27" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C27" s="11"/>
       <c r="D27" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E27" s="1">
         <v>17</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H27" s="1">
         <v>16</v>
@@ -1335,16 +1361,16 @@
     <row r="28" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C28" s="11"/>
       <c r="D28" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E28" s="1">
         <v>18</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H28" s="1">
         <v>17</v>
@@ -1375,16 +1401,16 @@
     <row r="29" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C29" s="11"/>
       <c r="D29" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E29" s="1">
         <v>19</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H29" s="1">
         <v>19</v>
@@ -1415,16 +1441,16 @@
     <row r="30" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C30" s="11"/>
       <c r="D30" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E30" s="1">
         <v>20</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H30" s="1">
         <v>16</v>

</xml_diff>

<commit_message>
Reading of the DAGMM paper
</commit_message>
<xml_diff>
--- a/ReadState.xlsx
+++ b/ReadState.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giamberm\Documents\TI\paper\2_Anomalie-detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DB4BA2-4866-4E40-BC69-32C7994C5E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1822D5E-3BD7-4DF2-96A9-42DFC3541884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +612,7 @@
       </c>
       <c r="I7" s="3">
         <f ca="1">NOW()</f>
-        <v>45377.426842245368</v>
+        <v>45377.58327314815</v>
       </c>
     </row>
     <row r="8" spans="3:17" x14ac:dyDescent="0.25">
@@ -1101,11 +1101,15 @@
         <f t="shared" si="0"/>
         <v>2.6367245372966863E-2</v>
       </c>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
+      <c r="L21" s="3">
+        <v>45377.504502314812</v>
+      </c>
+      <c r="M21" s="3">
+        <v>45377.583273032411</v>
+      </c>
       <c r="N21" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.8770717598672491E-2</v>
       </c>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>

</xml_diff>

<commit_message>
Readthrough : TCN vs LSTM (Gopali et al.  2021)
</commit_message>
<xml_diff>
--- a/ReadState.xlsx
+++ b/ReadState.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giamberm\Documents\TI\paper\2_Anomalie-detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA9CB33-EE0D-4409-BF4F-90F112919DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B349563-7E5F-4C86-9B66-49C7388E9F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
   <si>
     <t>Start</t>
   </si>
@@ -68,45 +68,12 @@
     <t>Toward the automation of mechanized tunneling</t>
   </si>
   <si>
-    <t>A Review of Time-Series Anomaly Detection Techniques - 2021 - K. Shaukat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anomaly Detection on Time Serie - 2010 -  Mingyan Teng </t>
-  </si>
-  <si>
-    <t>Anomaly Detection and Time Series Analysis -2023 - Ayush Anand</t>
-  </si>
-  <si>
-    <t>Multimedia datasets for anomaly detection: a review - 2023 - Pratibha Kumari</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An Experimental Evaluation of Time Series Classiﬁcation - 2018 - Górecki </t>
-  </si>
-  <si>
-    <t xml:space="preserve">An exhaustive comparison of distance measures in the classification of time series with 1NN method - 2024 - Górecki </t>
-  </si>
-  <si>
     <t xml:space="preserve">A SURVEY OF RESEARCH ON ANOMALY DETECTION FOR TIME SERIES  - 2016 - U-SHENG WU </t>
   </si>
   <si>
     <t>#pages</t>
   </si>
   <si>
-    <t>An Experimental Evaluation of Anomaly Detection in Time - 2023 - Zhang</t>
-  </si>
-  <si>
-    <t>DEEP AUTOENCODING GAUSSIAN MIXTURE MODEL FOR UNSUPERVISED ANOMALY DETECTION - 2018 - Zong</t>
-  </si>
-  <si>
-    <t>Unsupervised feature selection using chronological fitting with SHAP - 2024 - Quixuan</t>
-  </si>
-  <si>
-    <t>Anomaly detection in multivariate time series of drilling data - 2024 - Altindal</t>
-  </si>
-  <si>
-    <t>Recursive Principal Component Analysis-Based Data Outlier Detection - 2017 - Yu</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -140,21 +107,9 @@
     <t>-</t>
   </si>
   <si>
-    <t>A survey on anomaly detection for technical systems using LSTM networks - 2021 - Lindemann</t>
-  </si>
-  <si>
-    <t>Autoencoders for unsupervised anomaly segmentation in brain MR images: A comparative study - 2021 - Baur</t>
-  </si>
-  <si>
     <t xml:space="preserve">A deep hypersphere approach to high-dimensional anomaly detection - 2022 - Zheng </t>
   </si>
   <si>
-    <t>Real-time big data processing for anomaly detection: A Survey - Ahamed - 2019</t>
-  </si>
-  <si>
-    <t>A deep encoder-decoder network for anomaly detection - 2022 - Yu</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -176,16 +131,64 @@
     <t>Yes, relevant</t>
   </si>
   <si>
-    <t xml:space="preserve">Deep Learning for Anomaly Detection in Time-Series Data - 2021 - Choi </t>
-  </si>
-  <si>
-    <t>Pyramid reconstruction assisted deep autoencoding Gaussian mixture model for industrial fault detection - 2023 - Tian</t>
-  </si>
-  <si>
     <t>TCN</t>
   </si>
   <si>
-    <t>An Empirical Evaluation of Generic Convolutional and Recurrent Networks - Bai 2018</t>
+    <t xml:space="preserve">An Empirical Evaluation of Generic Convolutional and Recurrent Networks - Bai  et al.  2018 </t>
+  </si>
+  <si>
+    <t>A Comparison of TCN and LSTM Models in Detecting Anomalies in Time Series Data - Gopali et al.  2021</t>
+  </si>
+  <si>
+    <t>A deep encoder-decoder network for anomaly detection -  Yu et al. 2022</t>
+  </si>
+  <si>
+    <t>Real-time big data processing for anomaly detection: A Survey  - 2019 Ahamed et al.</t>
+  </si>
+  <si>
+    <t>Autoencoders for unsupervised anomaly segmentation in brain MR images: A comparative study - Baur et .al 2021</t>
+  </si>
+  <si>
+    <t>A survey on anomaly detection for technical systems using LSTM networks - Lindemann et al. 2021</t>
+  </si>
+  <si>
+    <t>Recursive Principal Component Analysis-Based Data Outlier Detection -  Yu et al. 2017</t>
+  </si>
+  <si>
+    <t>Anomaly detection in multivariate time series of drilling data - Altindal et al. 2024</t>
+  </si>
+  <si>
+    <t>Unsupervised feature selection using chronological fitting with SHAP - Quixuan et al. 2024</t>
+  </si>
+  <si>
+    <t>Pyramid reconstruction assisted deep autoencoding Gaussian mixture model for industrial fault detection - Tian et al. 2023</t>
+  </si>
+  <si>
+    <t>DEEP AUTOENCODING GAUSSIAN MIXTURE MODEL FOR UNSUPERVISED ANOMALY DETECTION - Zong et al. 2018</t>
+  </si>
+  <si>
+    <t>An Experimental Evaluation of Anomaly Detection in Time -  Zhang et al. 2023</t>
+  </si>
+  <si>
+    <t>Deep Learning for Anomaly Detection in Time-Series Data - Choi et al. 2021</t>
+  </si>
+  <si>
+    <t>An exhaustive comparison of distance measures in the classification of time series with 1NN method - Górecki et al. 2024</t>
+  </si>
+  <si>
+    <t>An Experimental Evaluation of Time Series Classiﬁcation - Górecki et al. 2018</t>
+  </si>
+  <si>
+    <t>Multimedia datasets for anomaly detection: a review -  Kumari et al 2023</t>
+  </si>
+  <si>
+    <t>Anomaly Detection and Time Series Analysis - Anand et al. 2023</t>
+  </si>
+  <si>
+    <t>A Review of Time-Series Anomaly Detection Techniques - K. Shaukat et al. 2021</t>
+  </si>
+  <si>
+    <t>Anomaly Detection on Time Serie - Teng  et al. 2010</t>
   </si>
 </sst>
 </file>
@@ -425,10 +428,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$I$23:$I$43</c:f>
+              <c:f>Tabelle1!$I$23:$I$60</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy\ h:mm</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>45362.4377662037</c:v>
                 </c:pt>
@@ -491,16 +494,19 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>45378.353567013888</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>45378.380602430552</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$K$23:$K$43</c:f>
+              <c:f>Tabelle1!$K$23:$K$60</c:f>
               <c:numCache>
                 <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>2.9161342594306916E-2</c:v>
                 </c:pt>
@@ -563,6 +569,57 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>6.5217592564295046E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.0624421302054543E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -624,7 +681,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1683,8 +1740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,7 +1750,7 @@
     <col min="3" max="3" width="64.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="107.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="112" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" style="1" customWidth="1"/>
     <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.42578125" style="1" customWidth="1"/>
@@ -1752,40 +1809,40 @@
     </row>
     <row r="17" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F17" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="G17" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F18" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="G18" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F19" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="G19" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="I19" s="3">
         <f ca="1">NOW()</f>
-        <v>45378.366239930554</v>
+        <v>45378.393694907405</v>
       </c>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F20" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C21" s="7" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D21" s="1">
         <f>COUNTIF(D23:D1012,D23)</f>
@@ -1807,22 +1864,22 @@
     </row>
     <row r="22" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>0</v>
@@ -1854,16 +1911,16 @@
     </row>
     <row r="23" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="11" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E23" s="1">
         <v>1</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>9</v>
@@ -1875,7 +1932,7 @@
         <v>45362.466927546295</v>
       </c>
       <c r="K23" s="4">
-        <f t="shared" ref="K23:K43" si="0">J23-I23</f>
+        <f t="shared" ref="K23:K60" si="0">J23-I23</f>
         <v>2.9161342594306916E-2</v>
       </c>
       <c r="L23" s="3"/>
@@ -1894,16 +1951,16 @@
     <row r="24" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C24" s="11"/>
       <c r="D24" s="6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E24" s="1">
         <v>2</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="I24" s="3">
         <v>45362.588587962964</v>
@@ -1918,7 +1975,7 @@
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="4">
-        <f t="shared" ref="N24:N43" si="1">M24-L24</f>
+        <f t="shared" ref="N24:N60" si="1">M24-L24</f>
         <v>0</v>
       </c>
       <c r="O24" s="3"/>
@@ -1931,16 +1988,16 @@
     <row r="25" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C25" s="11"/>
       <c r="D25" s="6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E25" s="1">
         <v>3</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="I25" s="3">
         <v>45362.637543171295</v>
@@ -1968,16 +2025,16 @@
     <row r="26" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C26" s="11"/>
       <c r="D26" s="6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E26" s="1">
         <v>4</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="I26" s="3">
         <v>45362.651693402775</v>
@@ -2009,16 +2066,16 @@
     <row r="27" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C27" s="11"/>
       <c r="D27" s="6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E27" s="1">
         <v>5</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="I27" s="3">
         <v>45363.563067129631</v>
@@ -2039,23 +2096,23 @@
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
       <c r="Q27" s="4">
-        <f t="shared" ref="Q27:Q43" si="3">P27-O27</f>
+        <f t="shared" ref="Q27:Q60" si="3">P27-O27</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C28" s="11"/>
       <c r="D28" s="6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E28" s="1">
         <v>6</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="I28" s="3">
         <v>45363.602375462964</v>
@@ -2083,14 +2140,14 @@
     <row r="29" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C29" s="11"/>
       <c r="D29" s="6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E29" s="1">
         <v>7</v>
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="8" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="I29" s="3">
         <v>45363.665852314814</v>
@@ -2118,16 +2175,16 @@
     <row r="30" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C30" s="11"/>
       <c r="D30" s="6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E30" s="1">
         <v>8</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H30" s="1">
         <v>6</v>
@@ -2158,16 +2215,16 @@
     <row r="31" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C31" s="11"/>
       <c r="D31" s="6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E31" s="1">
         <v>9</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H31" s="1">
         <v>23</v>
@@ -2183,7 +2240,7 @@
         <v>3.2596875003946479E-2</v>
       </c>
       <c r="L31" s="12" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="M31" s="12"/>
       <c r="N31" s="4" t="e">
@@ -2200,16 +2257,16 @@
     <row r="32" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C32" s="11"/>
       <c r="D32" s="6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E32" s="1">
         <v>10</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="H32" s="1">
         <v>14</v>
@@ -2240,16 +2297,16 @@
     <row r="33" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C33" s="6"/>
       <c r="D33" s="6" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E33" s="1">
         <v>11</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="H33" s="1">
         <v>19</v>
@@ -2284,16 +2341,16 @@
     <row r="34" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C34" s="6"/>
       <c r="D34" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E34" s="1">
         <v>12</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H34" s="1">
         <v>26</v>
@@ -2323,19 +2380,19 @@
     </row>
     <row r="35" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C35" s="11" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E35" s="1">
         <v>13</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H35" s="1">
         <v>18</v>
@@ -2366,16 +2423,16 @@
     <row r="36" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C36" s="11"/>
       <c r="D36" s="6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E36" s="1">
         <v>14</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="H36" s="1">
         <v>21</v>
@@ -2406,16 +2463,16 @@
     <row r="37" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C37" s="11"/>
       <c r="D37" s="6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E37" s="1">
         <v>15</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="H37" s="1">
         <v>10</v>
@@ -2445,19 +2502,19 @@
     </row>
     <row r="38" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C38" s="11" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E38" s="1">
         <v>16</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H38" s="1">
         <v>11</v>
@@ -2488,16 +2545,16 @@
     <row r="39" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C39" s="11"/>
       <c r="D39" s="6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E39" s="1">
         <v>17</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H39" s="1">
         <v>16</v>
@@ -2528,16 +2585,16 @@
     <row r="40" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C40" s="11"/>
       <c r="D40" s="6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E40" s="1">
         <v>18</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="H40" s="1">
         <v>17</v>
@@ -2568,16 +2625,16 @@
     <row r="41" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C41" s="11"/>
       <c r="D41" s="6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E41" s="1">
         <v>19</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H41" s="1">
         <v>19</v>
@@ -2608,16 +2665,16 @@
     <row r="42" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C42" s="11"/>
       <c r="D42" s="6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E42" s="1">
         <v>20</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H42" s="1">
         <v>16</v>
@@ -2647,16 +2704,16 @@
     </row>
     <row r="43" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D43" s="6" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="E43" s="1">
         <v>21</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="H43" s="1">
         <v>14</v>
@@ -2685,142 +2742,413 @@
       </c>
     </row>
     <row r="44" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
+      <c r="D44" t="s">
+        <v>31</v>
+      </c>
+      <c r="E44" s="1">
+        <v>22</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H44" s="1">
+        <v>6</v>
+      </c>
+      <c r="I44" s="3">
+        <v>45378.380602430552</v>
+      </c>
+      <c r="J44" s="3">
+        <v>45378.391226851854</v>
+      </c>
+      <c r="K44" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0624421302054543E-2</v>
+      </c>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
+      <c r="N44" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
+      <c r="Q44" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="E45" s="1">
+        <v>23</v>
+      </c>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
+      <c r="K45" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
+      <c r="N45" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
+      <c r="Q45" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="E46" s="1">
+        <v>24</v>
+      </c>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
+      <c r="K46" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
+      <c r="N46" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
+      <c r="Q46" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="E47" s="1">
+        <v>25</v>
+      </c>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
+      <c r="K47" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
+      <c r="N47" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
+      <c r="Q47" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="E48" s="1">
+        <v>26</v>
+      </c>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
+      <c r="K48" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
+      <c r="N48" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
-    </row>
-    <row r="49" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="Q48" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E49" s="1">
+        <v>27</v>
+      </c>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
+      <c r="K49" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
+      <c r="N49" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O49" s="3"/>
       <c r="P49" s="3"/>
-    </row>
-    <row r="50" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="Q49" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E50" s="1">
+        <v>28</v>
+      </c>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
+      <c r="K50" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
+      <c r="N50" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
-    </row>
-    <row r="51" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="Q50" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E51" s="1">
+        <v>29</v>
+      </c>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
+      <c r="K51" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
+      <c r="N51" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
-    </row>
-    <row r="52" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="Q51" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E52" s="1">
+        <v>30</v>
+      </c>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
+      <c r="K52" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
+      <c r="N52" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
-    </row>
-    <row r="53" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="Q52" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E53" s="1">
+        <v>31</v>
+      </c>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
+      <c r="K53" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
+      <c r="N53" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
-    </row>
-    <row r="54" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="Q53" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E54" s="1">
+        <v>32</v>
+      </c>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
+      <c r="K54" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
+      <c r="N54" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O54" s="3"/>
       <c r="P54" s="3"/>
-    </row>
-    <row r="55" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="Q54" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E55" s="1">
+        <v>33</v>
+      </c>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
+      <c r="K55" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
+      <c r="N55" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O55" s="3"/>
       <c r="P55" s="3"/>
-    </row>
-    <row r="56" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="Q55" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E56" s="1">
+        <v>34</v>
+      </c>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
+      <c r="K56" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
+      <c r="N56" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O56" s="3"/>
       <c r="P56" s="3"/>
-    </row>
-    <row r="57" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="Q56" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E57" s="1">
+        <v>35</v>
+      </c>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
+      <c r="K57" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
+      <c r="N57" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O57" s="3"/>
       <c r="P57" s="3"/>
-    </row>
-    <row r="58" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="Q57" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E58" s="1">
+        <v>36</v>
+      </c>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
+      <c r="K58" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
+      <c r="N58" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O58" s="3"/>
       <c r="P58" s="3"/>
-    </row>
-    <row r="59" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="Q58" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E59" s="1">
+        <v>37</v>
+      </c>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
+      <c r="K59" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
+      <c r="N59" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O59" s="3"/>
       <c r="P59" s="3"/>
-    </row>
-    <row r="60" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="Q59" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E60" s="1">
+        <v>38</v>
+      </c>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
+      <c r="K60" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L60" s="3"/>
       <c r="M60" s="3"/>
+      <c r="N60" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O60" s="3"/>
       <c r="P60" s="3"/>
-    </row>
-    <row r="61" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="Q60" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
       <c r="L61" s="3"/>
@@ -2828,7 +3156,7 @@
       <c r="O61" s="3"/>
       <c r="P61" s="3"/>
     </row>
-    <row r="62" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
       <c r="L62" s="3"/>
@@ -2836,7 +3164,7 @@
       <c r="O62" s="3"/>
       <c r="P62" s="3"/>
     </row>
-    <row r="63" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
       <c r="L63" s="3"/>
@@ -2844,7 +3172,7 @@
       <c r="O63" s="3"/>
       <c r="P63" s="3"/>
     </row>
-    <row r="64" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
       <c r="L64" s="3"/>

</xml_diff>

<commit_message>
Readthrough : Core loss (Shang et al. 2023)
</commit_message>
<xml_diff>
--- a/ReadState.xlsx
+++ b/ReadState.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giamberm\Documents\TI\paper\2_Anomalie-detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B349563-7E5F-4C86-9B66-49C7388E9F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C9903B-279B-4DF4-93FE-5A7F8DBFE914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
   <si>
     <t>Start</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>Anomaly Detection on Time Serie - Teng  et al. 2010</t>
+  </si>
+  <si>
+    <t>Core loss: Mining core samples efficiently for robust machine anomaly detection against data pollution - Shang et al. 2023</t>
   </si>
 </sst>
 </file>
@@ -498,6 +501,9 @@
                 <c:pt idx="21">
                   <c:v>45378.380602430552</c:v>
                 </c:pt>
+                <c:pt idx="22">
+                  <c:v>45378.410335069442</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -574,7 +580,7 @@
                   <c:v>1.0624421302054543E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>1.4993055556260515E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>0</c:v>
@@ -1740,8 +1746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1832,7 +1838,7 @@
       </c>
       <c r="I19" s="3">
         <f ca="1">NOW()</f>
-        <v>45378.393694907405</v>
+        <v>45378.425328472222</v>
       </c>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.25">
@@ -2784,11 +2790,21 @@
       <c r="E45" s="1">
         <v>23</v>
       </c>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
+      <c r="G45" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H45" s="1">
+        <v>17</v>
+      </c>
+      <c r="I45" s="3">
+        <v>45378.410335069442</v>
+      </c>
+      <c r="J45" s="3">
+        <v>45378.425328124998</v>
+      </c>
       <c r="K45" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.4993055556260515E-2</v>
       </c>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>

</xml_diff>

<commit_message>
1st Readthrough : LOE Qiu et al. 2022
</commit_message>
<xml_diff>
--- a/ReadState.xlsx
+++ b/ReadState.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giamberm\Documents\TI\paper\2_Anomalie-detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C9903B-279B-4DF4-93FE-5A7F8DBFE914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFC1AE7-B47B-4865-974D-7599E1FE5D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="55">
   <si>
     <t>Start</t>
   </si>
@@ -192,6 +192,15 @@
   </si>
   <si>
     <t>Core loss: Mining core samples efficiently for robust machine anomaly detection against data pollution - Shang et al. 2023</t>
+  </si>
+  <si>
+    <t>Anomaly detection unsupervised with contamination</t>
+  </si>
+  <si>
+    <t>Bulk</t>
+  </si>
+  <si>
+    <t>Latent Outlier Exposure for Anomaly Detection with Contaminated Data - Qiu et al. 2022</t>
   </si>
 </sst>
 </file>
@@ -504,6 +513,9 @@
                 <c:pt idx="22">
                   <c:v>45378.410335069442</c:v>
                 </c:pt>
+                <c:pt idx="23">
+                  <c:v>45378.645685763891</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -583,7 +595,7 @@
                   <c:v>1.4993055556260515E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>1.2545254627184477E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>0</c:v>
@@ -1746,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1838,7 +1850,7 @@
       </c>
       <c r="I19" s="3">
         <f ca="1">NOW()</f>
-        <v>45378.425328472222</v>
+        <v>45378.658557523151</v>
       </c>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.25">
@@ -2790,6 +2802,9 @@
       <c r="E45" s="1">
         <v>23</v>
       </c>
+      <c r="F45" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="G45" s="8" t="s">
         <v>51</v>
       </c>
@@ -2820,14 +2835,33 @@
       </c>
     </row>
     <row r="46" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C46" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="E46" s="1">
         <v>24</v>
       </c>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
+      <c r="F46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H46" s="1">
+        <v>15</v>
+      </c>
+      <c r="I46" s="3">
+        <v>45378.645685763891</v>
+      </c>
+      <c r="J46" s="3">
+        <v>45378.658231018519</v>
+      </c>
       <c r="K46" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.2545254627184477E-2</v>
       </c>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
@@ -2843,6 +2877,10 @@
       </c>
     </row>
     <row r="47" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C47" s="11"/>
+      <c r="D47" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="E47" s="1">
         <v>25</v>
       </c>
@@ -2866,6 +2904,10 @@
       </c>
     </row>
     <row r="48" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C48" s="11"/>
+      <c r="D48" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="E48" s="1">
         <v>26</v>
       </c>
@@ -2888,7 +2930,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C49" s="11"/>
+      <c r="D49" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="E49" s="1">
         <v>27</v>
       </c>
@@ -2911,7 +2957,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C50" s="11"/>
+      <c r="D50" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="E50" s="1">
         <v>28</v>
       </c>
@@ -2934,7 +2984,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C51" s="11"/>
+      <c r="D51" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="E51" s="1">
         <v>29</v>
       </c>
@@ -2957,7 +3011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E52" s="1">
         <v>30</v>
       </c>
@@ -2980,7 +3034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E53" s="1">
         <v>31</v>
       </c>
@@ -3003,7 +3057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E54" s="1">
         <v>32</v>
       </c>
@@ -3026,7 +3080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E55" s="1">
         <v>33</v>
       </c>
@@ -3049,7 +3103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E56" s="1">
         <v>34</v>
       </c>
@@ -3072,7 +3126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E57" s="1">
         <v>35</v>
       </c>
@@ -3095,7 +3149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E58" s="1">
         <v>36</v>
       </c>
@@ -3118,7 +3172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E59" s="1">
         <v>37</v>
       </c>
@@ -3141,7 +3195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E60" s="1">
         <v>38</v>
       </c>
@@ -3164,7 +3218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:17" x14ac:dyDescent="0.25">
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
       <c r="L61" s="3"/>
@@ -3172,7 +3226,7 @@
       <c r="O61" s="3"/>
       <c r="P61" s="3"/>
     </row>
-    <row r="62" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:17" x14ac:dyDescent="0.25">
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
       <c r="L62" s="3"/>
@@ -3180,7 +3234,7 @@
       <c r="O62" s="3"/>
       <c r="P62" s="3"/>
     </row>
-    <row r="63" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:17" x14ac:dyDescent="0.25">
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
       <c r="L63" s="3"/>
@@ -3188,7 +3242,7 @@
       <c r="O63" s="3"/>
       <c r="P63" s="3"/>
     </row>
-    <row r="64" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:17" x14ac:dyDescent="0.25">
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
       <c r="L64" s="3"/>
@@ -3205,7 +3259,8 @@
       <c r="P65" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="C46:C51"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="L21:M21"/>
     <mergeCell ref="O21:P21"/>

</xml_diff>

<commit_message>
1st Readthrough : Li et al. 2021
</commit_message>
<xml_diff>
--- a/ReadState.xlsx
+++ b/ReadState.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giamberm\Documents\TI\paper\2_Anomalie-detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFC1AE7-B47B-4865-974D-7599E1FE5D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9FFF5D-9F2B-4FE7-BF21-FBDB40FB6BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="57">
   <si>
     <t>Start</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>Latent Outlier Exposure for Anomaly Detection with Contaminated Data - Qiu et al. 2022</t>
+  </si>
+  <si>
+    <t>An Iterative Method for Unsupervised Robust Anomaly Detection under Data Contamination - Kim et al. 2021</t>
+  </si>
+  <si>
+    <t>Deep Unsupervised Anomaly Detection - Li et al. 2021</t>
   </si>
 </sst>
 </file>
@@ -516,6 +522,12 @@
                 <c:pt idx="23">
                   <c:v>45378.645685763891</c:v>
                 </c:pt>
+                <c:pt idx="24">
+                  <c:v>45378.666361342592</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>45378.686284722222</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -598,10 +610,10 @@
                   <c:v>1.2545254627184477E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>1.5405092592118308E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>4.2009259268525057E-3</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0</c:v>
@@ -1758,8 +1770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1850,7 +1862,7 @@
       </c>
       <c r="I19" s="3">
         <f ca="1">NOW()</f>
-        <v>45378.658557523151</v>
+        <v>45378.691784490744</v>
       </c>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.25">
@@ -2884,11 +2896,24 @@
       <c r="E47" s="1">
         <v>25</v>
       </c>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
+      <c r="F47" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H47" s="1">
+        <v>13</v>
+      </c>
+      <c r="I47" s="3">
+        <v>45378.666361342592</v>
+      </c>
+      <c r="J47" s="3">
+        <v>45378.681766435184</v>
+      </c>
       <c r="K47" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5405092592118308E-2</v>
       </c>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
@@ -2911,11 +2936,24 @@
       <c r="E48" s="1">
         <v>26</v>
       </c>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
+      <c r="F48" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H48" s="1">
+        <v>10</v>
+      </c>
+      <c r="I48" s="3">
+        <v>45378.686284722222</v>
+      </c>
+      <c r="J48" s="3">
+        <v>45378.690485648149</v>
+      </c>
       <c r="K48" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.2009259268525057E-3</v>
       </c>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>

</xml_diff>

<commit_message>
1st Readthrough : NegCo (Lin et al. 2024)
</commit_message>
<xml_diff>
--- a/ReadState.xlsx
+++ b/ReadState.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giamberm\Documents\TI\paper\2_Anomalie-detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9FFF5D-9F2B-4FE7-BF21-FBDB40FB6BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41674A2E-735E-4DB6-9DEE-B705AB34ACD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="59">
   <si>
     <t>Start</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>Deep Unsupervised Anomaly Detection - Li et al. 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploiting negative correlation for unsupervised anomaly detection in contaminated time series - Lin et al. 2024 </t>
+  </si>
+  <si>
+    <t>Unsupervised Time Series Anomaly Detection under Data Contamination - Xiaoguhi et al. 2022</t>
   </si>
 </sst>
 </file>
@@ -292,11 +298,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -528,6 +534,9 @@
                 <c:pt idx="25">
                   <c:v>45378.686284722222</c:v>
                 </c:pt>
+                <c:pt idx="26">
+                  <c:v>45379.335048148147</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -616,7 +625,7 @@
                   <c:v>4.2009259268525057E-3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>2.0674884261097759E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>0</c:v>
@@ -1770,8 +1779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1862,7 +1871,7 @@
       </c>
       <c r="I19" s="3">
         <f ca="1">NOW()</f>
-        <v>45378.691784490744</v>
+        <v>45379.35646747685</v>
       </c>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.25">
@@ -1879,18 +1888,18 @@
         <v>18</v>
       </c>
       <c r="G21"/>
-      <c r="I21" s="10" t="s">
+      <c r="I21" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="J21" s="10"/>
-      <c r="L21" s="10" t="s">
+      <c r="J21" s="11"/>
+      <c r="L21" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="M21" s="10"/>
-      <c r="O21" s="10" t="s">
+      <c r="M21" s="11"/>
+      <c r="O21" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="P21" s="10"/>
+      <c r="P21" s="11"/>
     </row>
     <row r="22" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
@@ -1940,7 +1949,7 @@
       </c>
     </row>
     <row r="23" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>18</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -1979,7 +1988,7 @@
       </c>
     </row>
     <row r="24" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C24" s="11"/>
+      <c r="C24" s="10"/>
       <c r="D24" s="6" t="s">
         <v>15</v>
       </c>
@@ -2016,7 +2025,7 @@
       </c>
     </row>
     <row r="25" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C25" s="11"/>
+      <c r="C25" s="10"/>
       <c r="D25" s="6" t="s">
         <v>15</v>
       </c>
@@ -2053,7 +2062,7 @@
       </c>
     </row>
     <row r="26" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C26" s="11"/>
+      <c r="C26" s="10"/>
       <c r="D26" s="6" t="s">
         <v>15</v>
       </c>
@@ -2094,7 +2103,7 @@
       </c>
     </row>
     <row r="27" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C27" s="11"/>
+      <c r="C27" s="10"/>
       <c r="D27" s="6" t="s">
         <v>15</v>
       </c>
@@ -2131,14 +2140,14 @@
       </c>
     </row>
     <row r="28" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C28" s="11"/>
+      <c r="C28" s="10"/>
       <c r="D28" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E28" s="1">
         <v>6</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F28" s="10" t="s">
         <v>24</v>
       </c>
       <c r="G28" s="8" t="s">
@@ -2168,14 +2177,14 @@
       </c>
     </row>
     <row r="29" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C29" s="11"/>
+      <c r="C29" s="10"/>
       <c r="D29" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E29" s="1">
         <v>7</v>
       </c>
-      <c r="F29" s="11"/>
+      <c r="F29" s="10"/>
       <c r="G29" s="8" t="s">
         <v>45</v>
       </c>
@@ -2203,7 +2212,7 @@
       </c>
     </row>
     <row r="30" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C30" s="11"/>
+      <c r="C30" s="10"/>
       <c r="D30" s="6" t="s">
         <v>15</v>
       </c>
@@ -2243,7 +2252,7 @@
       </c>
     </row>
     <row r="31" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C31" s="11"/>
+      <c r="C31" s="10"/>
       <c r="D31" s="6" t="s">
         <v>15</v>
       </c>
@@ -2285,7 +2294,7 @@
       </c>
     </row>
     <row r="32" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C32" s="11"/>
+      <c r="C32" s="10"/>
       <c r="D32" s="6" t="s">
         <v>15</v>
       </c>
@@ -2409,7 +2418,7 @@
       </c>
     </row>
     <row r="35" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D35" s="6" t="s">
@@ -2451,7 +2460,7 @@
       </c>
     </row>
     <row r="36" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C36" s="11"/>
+      <c r="C36" s="10"/>
       <c r="D36" s="6" t="s">
         <v>15</v>
       </c>
@@ -2491,7 +2500,7 @@
       </c>
     </row>
     <row r="37" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C37" s="11"/>
+      <c r="C37" s="10"/>
       <c r="D37" s="6" t="s">
         <v>15</v>
       </c>
@@ -2531,7 +2540,7 @@
       </c>
     </row>
     <row r="38" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="10" t="s">
         <v>20</v>
       </c>
       <c r="D38" s="6" t="s">
@@ -2573,7 +2582,7 @@
       </c>
     </row>
     <row r="39" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C39" s="11"/>
+      <c r="C39" s="10"/>
       <c r="D39" s="6" t="s">
         <v>15</v>
       </c>
@@ -2613,7 +2622,7 @@
       </c>
     </row>
     <row r="40" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C40" s="11"/>
+      <c r="C40" s="10"/>
       <c r="D40" s="6" t="s">
         <v>15</v>
       </c>
@@ -2653,7 +2662,7 @@
       </c>
     </row>
     <row r="41" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C41" s="11"/>
+      <c r="C41" s="10"/>
       <c r="D41" s="6" t="s">
         <v>15</v>
       </c>
@@ -2693,7 +2702,7 @@
       </c>
     </row>
     <row r="42" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C42" s="11"/>
+      <c r="C42" s="10"/>
       <c r="D42" s="6" t="s">
         <v>15</v>
       </c>
@@ -2847,7 +2856,7 @@
       </c>
     </row>
     <row r="46" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="10" t="s">
         <v>52</v>
       </c>
       <c r="D46" s="6" t="s">
@@ -2889,7 +2898,7 @@
       </c>
     </row>
     <row r="47" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C47" s="11"/>
+      <c r="C47" s="10"/>
       <c r="D47" s="6" t="s">
         <v>53</v>
       </c>
@@ -2929,7 +2938,7 @@
       </c>
     </row>
     <row r="48" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C48" s="11"/>
+      <c r="C48" s="10"/>
       <c r="D48" s="6" t="s">
         <v>53</v>
       </c>
@@ -2969,18 +2978,31 @@
       </c>
     </row>
     <row r="49" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C49" s="11"/>
+      <c r="C49" s="10"/>
       <c r="D49" s="6" t="s">
         <v>53</v>
       </c>
       <c r="E49" s="1">
         <v>27</v>
       </c>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
+      <c r="F49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H49" s="1">
+        <v>11</v>
+      </c>
+      <c r="I49" s="3">
+        <v>45379.335048148147</v>
+      </c>
+      <c r="J49" s="3">
+        <v>45379.355723032408</v>
+      </c>
       <c r="K49" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0674884261097759E-2</v>
       </c>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
@@ -2996,12 +3018,15 @@
       </c>
     </row>
     <row r="50" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C50" s="11"/>
+      <c r="C50" s="10"/>
       <c r="D50" s="6" t="s">
         <v>53</v>
       </c>
       <c r="E50" s="1">
         <v>28</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
@@ -3023,7 +3048,7 @@
       </c>
     </row>
     <row r="51" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C51" s="11"/>
+      <c r="C51" s="10"/>
       <c r="D51" s="6" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
2nd Readthrought TCN Bai  et al.  2018
</commit_message>
<xml_diff>
--- a/ReadState.xlsx
+++ b/ReadState.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giamberm\Documents\TI\paper\2_Anomalie-detection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Documents\Cours\KIT\11_HK\AD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9802517-1DC9-4B59-B971-7A4B8FCDFBE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499E119A-BB73-4813-ACA1-F3F06AAEEEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1782,74 +1782,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="F19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.109375" style="1"/>
     <col min="7" max="7" width="112" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" style="1" customWidth="1"/>
-    <col min="12" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" style="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" style="1" customWidth="1"/>
+    <col min="12" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G1"/>
     </row>
-    <row r="2" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G2"/>
     </row>
-    <row r="3" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G3"/>
     </row>
-    <row r="4" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G4"/>
     </row>
-    <row r="5" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G5"/>
     </row>
-    <row r="6" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G6"/>
     </row>
-    <row r="7" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G7"/>
     </row>
-    <row r="8" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G8"/>
     </row>
-    <row r="9" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G9"/>
     </row>
-    <row r="10" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G10"/>
     </row>
-    <row r="11" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G11"/>
     </row>
-    <row r="12" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G12"/>
     </row>
-    <row r="13" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G13"/>
     </row>
-    <row r="14" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G14"/>
     </row>
-    <row r="15" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G15"/>
     </row>
-    <row r="16" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G16"/>
     </row>
-    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:17" x14ac:dyDescent="0.3">
       <c r="F17" s="1" t="s">
         <v>25</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:17" x14ac:dyDescent="0.3">
       <c r="F18" s="1" t="s">
         <v>26</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:17" x14ac:dyDescent="0.3">
       <c r="F19" s="1" t="s">
         <v>24</v>
       </c>
@@ -1874,15 +1874,15 @@
       </c>
       <c r="I19" s="3">
         <f ca="1">NOW()</f>
-        <v>45379.438686689813</v>
-      </c>
-    </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
+        <v>45443.569031018516</v>
+      </c>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.3">
       <c r="F20" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C21" s="7" t="s">
         <v>14</v>
       </c>
@@ -1904,7 +1904,7 @@
       </c>
       <c r="P21" s="11"/>
     </row>
-    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C22" s="2" t="s">
         <v>17</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="10" t="s">
         <v>18</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C24" s="10"/>
       <c r="D24" s="6" t="s">
         <v>15</v>
@@ -2027,7 +2027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C25" s="10"/>
       <c r="D25" s="6" t="s">
         <v>15</v>
@@ -2064,7 +2064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C26" s="10"/>
       <c r="D26" s="6" t="s">
         <v>15</v>
@@ -2105,7 +2105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C27" s="10"/>
       <c r="D27" s="6" t="s">
         <v>15</v>
@@ -2142,7 +2142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C28" s="10"/>
       <c r="D28" s="6" t="s">
         <v>15</v>
@@ -2179,7 +2179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C29" s="10"/>
       <c r="D29" s="6" t="s">
         <v>15</v>
@@ -2214,7 +2214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C30" s="10"/>
       <c r="D30" s="6" t="s">
         <v>15</v>
@@ -2254,7 +2254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C31" s="10"/>
       <c r="D31" s="6" t="s">
         <v>15</v>
@@ -2296,7 +2296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C32" s="10"/>
       <c r="D32" s="6" t="s">
         <v>15</v>
@@ -2336,7 +2336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C33" s="6"/>
       <c r="D33" s="6" t="s">
         <v>16</v>
@@ -2380,7 +2380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C34" s="6"/>
       <c r="D34" t="s">
         <v>16</v>
@@ -2420,7 +2420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C35" s="10" t="s">
         <v>19</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C36" s="10"/>
       <c r="D36" s="6" t="s">
         <v>15</v>
@@ -2502,7 +2502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C37" s="10"/>
       <c r="D37" s="6" t="s">
         <v>15</v>
@@ -2542,7 +2542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C38" s="10" t="s">
         <v>20</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C39" s="10"/>
       <c r="D39" s="6" t="s">
         <v>15</v>
@@ -2624,7 +2624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C40" s="10"/>
       <c r="D40" s="6" t="s">
         <v>15</v>
@@ -2664,7 +2664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C41" s="10"/>
       <c r="D41" s="6" t="s">
         <v>15</v>
@@ -2704,7 +2704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C42" s="10"/>
       <c r="D42" s="6" t="s">
         <v>15</v>
@@ -2744,7 +2744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D43" s="6" t="s">
         <v>31</v>
       </c>
@@ -2770,11 +2770,15 @@
         <f t="shared" si="0"/>
         <v>6.5217592564295046E-3</v>
       </c>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
+      <c r="L43" s="3">
+        <v>45443.521180555559</v>
+      </c>
+      <c r="M43" s="3">
+        <v>45443.569030902778</v>
+      </c>
       <c r="N43" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.7850347218627576E-2</v>
       </c>
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
@@ -2783,7 +2787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
         <v>31</v>
       </c>
@@ -2822,7 +2826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E45" s="1">
         <v>23</v>
       </c>
@@ -2858,7 +2862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C46" s="10" t="s">
         <v>52</v>
       </c>
@@ -2900,7 +2904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C47" s="10"/>
       <c r="D47" s="6" t="s">
         <v>53</v>
@@ -2940,7 +2944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C48" s="10"/>
       <c r="D48" s="6" t="s">
         <v>53</v>
@@ -2980,7 +2984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C49" s="10"/>
       <c r="D49" s="6" t="s">
         <v>53</v>
@@ -3020,7 +3024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C50" s="10"/>
       <c r="D50" s="6" t="s">
         <v>53</v>
@@ -3060,7 +3064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C51" s="10"/>
       <c r="D51" s="6" t="s">
         <v>53</v>
@@ -3087,7 +3091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E52" s="1">
         <v>30</v>
       </c>
@@ -3110,7 +3114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E53" s="1">
         <v>31</v>
       </c>
@@ -3133,7 +3137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E54" s="1">
         <v>32</v>
       </c>
@@ -3156,7 +3160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E55" s="1">
         <v>33</v>
       </c>
@@ -3179,7 +3183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E56" s="1">
         <v>34</v>
       </c>
@@ -3202,7 +3206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E57" s="1">
         <v>35</v>
       </c>
@@ -3225,7 +3229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E58" s="1">
         <v>36</v>
       </c>
@@ -3248,7 +3252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E59" s="1">
         <v>37</v>
       </c>
@@ -3271,7 +3275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E60" s="1">
         <v>38</v>
       </c>
@@ -3294,7 +3298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:17" x14ac:dyDescent="0.3">
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
       <c r="L61" s="3"/>
@@ -3302,7 +3306,7 @@
       <c r="O61" s="3"/>
       <c r="P61" s="3"/>
     </row>
-    <row r="62" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:17" x14ac:dyDescent="0.3">
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
       <c r="L62" s="3"/>
@@ -3310,7 +3314,7 @@
       <c r="O62" s="3"/>
       <c r="P62" s="3"/>
     </row>
-    <row r="63" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:17" x14ac:dyDescent="0.3">
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
       <c r="L63" s="3"/>
@@ -3318,7 +3322,7 @@
       <c r="O63" s="3"/>
       <c r="P63" s="3"/>
     </row>
-    <row r="64" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:17" x14ac:dyDescent="0.3">
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
       <c r="L64" s="3"/>
@@ -3326,7 +3330,7 @@
       <c r="O64" s="3"/>
       <c r="P64" s="3"/>
     </row>
-    <row r="65" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="9:16" x14ac:dyDescent="0.3">
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="L65" s="3"/>

</xml_diff>

<commit_message>
Xianhang et al. - 2nd Readthrough
</commit_message>
<xml_diff>
--- a/ReadState.xlsx
+++ b/ReadState.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Documents\Cours\KIT\11_HK\AD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499E119A-BB73-4813-ACA1-F3F06AAEEEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABD52A3-73BD-4AFC-BFD4-AD5639DBD43E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="61">
   <si>
     <t>Start</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t>Unsupervised Time Series Anomaly Detection under Data Contamination - Xiaoguhi et al. 2022</t>
+  </si>
+  <si>
+    <t>Animaly detection and Fault Prognosis for bearings - Xiaohang et al. 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AR</t>
   </si>
 </sst>
 </file>
@@ -1782,8 +1788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M40" sqref="M40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1874,7 +1880,7 @@
       </c>
       <c r="I19" s="3">
         <f ca="1">NOW()</f>
-        <v>45443.569031018516</v>
+        <v>45467.690373958336</v>
       </c>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.3">
@@ -3065,12 +3071,21 @@
       </c>
     </row>
     <row r="51" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C51" s="10"/>
+      <c r="C51" s="6"/>
       <c r="D51" s="6" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E51" s="1">
         <v>29</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H51" s="1">
+        <v>10</v>
       </c>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
@@ -3078,11 +3093,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
+      <c r="L51" s="3">
+        <v>45467.665670254632</v>
+      </c>
+      <c r="M51" s="3">
+        <v>45467.689860300925</v>
+      </c>
       <c r="N51" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.419004629336996E-2</v>
       </c>
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
@@ -3340,7 +3359,6 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="C46:C51"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="L21:M21"/>
     <mergeCell ref="O21:P21"/>
@@ -3349,6 +3367,7 @@
     <mergeCell ref="C35:C37"/>
     <mergeCell ref="F28:F29"/>
     <mergeCell ref="L31:M31"/>
+    <mergeCell ref="C46:C50"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D23:D1012" xr:uid="{3C1CE3FE-DB2C-4C19-8BC4-C9EF203C546F}">

</xml_diff>

<commit_message>
Deng, Hooi 2021 -  1st Readthrough
</commit_message>
<xml_diff>
--- a/ReadState.xlsx
+++ b/ReadState.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Documents\Cours\KIT\11_HK\AD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABD52A3-73BD-4AFC-BFD4-AD5639DBD43E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CD4F0E-8FFC-4E0D-BAB7-461ED6A39B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="62">
   <si>
     <t>Start</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t xml:space="preserve"> AR</t>
+  </si>
+  <si>
+    <t>Graph Neural Network-Based Anomaly Detection in Multivariate Time Series - Ailin Deng, Bryan Hooi 2021</t>
   </si>
 </sst>
 </file>
@@ -546,6 +549,9 @@
                 <c:pt idx="27">
                   <c:v>45379.360102777777</c:v>
                 </c:pt>
+                <c:pt idx="29">
+                  <c:v>45467.711563657409</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -643,7 +649,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>1.0157523145608138E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>0</c:v>
@@ -1788,8 +1794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="D36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1880,7 +1886,7 @@
       </c>
       <c r="I19" s="3">
         <f ca="1">NOW()</f>
-        <v>45467.690373958336</v>
+        <v>45467.721725578704</v>
       </c>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.3">
@@ -3114,11 +3120,24 @@
       <c r="E52" s="1">
         <v>30</v>
       </c>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
+      <c r="F52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H52" s="1">
+        <v>9</v>
+      </c>
+      <c r="I52" s="3">
+        <v>45467.711563657409</v>
+      </c>
+      <c r="J52" s="3">
+        <v>45467.721721180555</v>
+      </c>
       <c r="K52" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.0157523145608138E-2</v>
       </c>
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>

</xml_diff>